<commit_message>
Now user can select multiple categories along with multiple selection, however currently equipment info page is in progress.
</commit_message>
<xml_diff>
--- a/ATMAgreementWizard/ExcelData/sample.xlsx
+++ b/ATMAgreementWizard/ExcelData/sample.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t xml:space="preserve">Username</t>
   </si>
@@ -54,6 +54,24 @@
     <t xml:space="preserve">10TH &amp; BANNOCK</t>
   </si>
   <si>
+    <t xml:space="preserve">def</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ghi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9TH AVE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FERNDALE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YAKIMA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">null</t>
+  </si>
+  <si>
     <t xml:space="preserve">Equipment Category</t>
   </si>
   <si>
@@ -73,9 +91,6 @@
   </si>
   <si>
     <t xml:space="preserve">Hosted Server Agreement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">null</t>
   </si>
 </sst>
 </file>
@@ -85,7 +100,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -124,11 +139,24 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF0000C0"/>
       <name val="Consolas"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -205,7 +233,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -226,7 +254,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -234,7 +266,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -242,10 +282,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -254,11 +290,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -391,13 +431,13 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="40.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.03"/>
@@ -414,10 +454,10 @@
       <c r="B1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="4"/>
+      <c r="D1" s="5"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
@@ -425,109 +465,121 @@
       <c r="I1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="6"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="10"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -548,7 +600,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -568,14 +620,14 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
-      <c r="E1" s="12"/>
+      <c r="E1" s="15"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
@@ -584,117 +636,117 @@
       <c r="K1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
+      <c r="A2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
+      <c r="A3" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>